<commit_message>
work on shock loop (with comments from Italo on 10/26), work on comparison between interpolations.
</commit_message>
<xml_diff>
--- a/ini_ss.xlsx
+++ b/ini_ss.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:M217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K38" sqref="H38:K38"/>
+      <selection activeCell="M188" sqref="M188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7511,41 +7511,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A188">
-        <v>1</v>
-      </c>
-      <c r="B188">
-        <v>1</v>
-      </c>
-      <c r="C188">
-        <v>3</v>
-      </c>
-      <c r="D188">
-        <v>3</v>
-      </c>
-      <c r="E188">
-        <v>3</v>
-      </c>
-      <c r="F188">
-        <v>1</v>
-      </c>
-      <c r="H188">
+    <row r="188" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="1">
+        <v>1</v>
+      </c>
+      <c r="B188" s="1">
+        <v>1</v>
+      </c>
+      <c r="C188" s="1">
+        <v>3</v>
+      </c>
+      <c r="D188" s="1">
+        <v>3</v>
+      </c>
+      <c r="E188" s="1">
+        <v>3</v>
+      </c>
+      <c r="F188" s="1">
+        <v>1</v>
+      </c>
+      <c r="H188" s="1">
         <v>16.225000000000001</v>
       </c>
-      <c r="I188">
-        <v>2</v>
-      </c>
-      <c r="J188">
-        <v>3</v>
-      </c>
-      <c r="K188">
-        <v>3</v>
-      </c>
-      <c r="L188">
-        <v>3</v>
-      </c>
-      <c r="M188">
+      <c r="I188" s="1">
+        <v>2</v>
+      </c>
+      <c r="J188" s="1">
+        <v>3</v>
+      </c>
+      <c r="K188" s="1">
+        <v>3</v>
+      </c>
+      <c r="L188" s="1">
+        <v>3</v>
+      </c>
+      <c r="M188" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>